<commit_message>
end dates Utrecht corrected
</commit_message>
<xml_diff>
--- a/utrecht.xlsx
+++ b/utrecht.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hldeb\PycharmProjects\meetjestad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{C6A585A6-D72F-4641-8085-ABF89321571D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2A63A4B0-EE10-41FA-A128-C772ED54849C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{2A448916-CE78-4DC2-8059-01F26DFA5170}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{063E4B95-7626-4A8E-B256-F67A4AB3E4B3}"/>
   </bookViews>
   <sheets>
     <sheet name="utrecht" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="17">
   <si>
     <t>ID</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>Maarssen</t>
+  </si>
+  <si>
+    <t>De Bilt</t>
   </si>
 </sst>
 </file>
@@ -942,19 +945,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEB556D0-F695-4CFB-90EF-6C69056951F2}">
-  <dimension ref="A1:L123"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E98003D5-2E2F-4FA8-A653-0ADF3AC6805A}">
+  <dimension ref="A1:P119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:L123"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="10.6640625" customWidth="1"/>
-    <col min="3" max="3" width="10.1328125" customWidth="1"/>
+    <col min="2" max="2" width="10.73046875" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" customWidth="1"/>
-    <col min="5" max="5" width="11.3984375" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.45">
@@ -1062,9 +1065,6 @@
       <c r="F5">
         <v>0</v>
       </c>
-      <c r="J5">
-        <v>154</v>
-      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6">
@@ -1086,7 +1086,7 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.45">
@@ -1108,11 +1108,8 @@
       <c r="F7">
         <v>0</v>
       </c>
-      <c r="K7" s="2">
-        <v>157</v>
-      </c>
-      <c r="L7" t="s">
-        <v>7</v>
+      <c r="J7">
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.45">
@@ -1137,6 +1134,12 @@
       <c r="J8">
         <v>159</v>
       </c>
+      <c r="K8" s="2">
+        <v>157</v>
+      </c>
+      <c r="L8" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9">
@@ -1277,6 +1280,9 @@
       <c r="D15" s="1">
         <v>44994</v>
       </c>
+      <c r="E15" s="1">
+        <v>45893</v>
+      </c>
       <c r="F15">
         <v>0</v>
       </c>
@@ -1392,111 +1398,111 @@
       <c r="F20">
         <v>0</v>
       </c>
+      <c r="K20" s="2">
+        <v>606</v>
+      </c>
+      <c r="L20" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A21">
-        <v>606</v>
+        <v>639</v>
       </c>
       <c r="B21" s="1">
-        <v>44562</v>
+        <v>45089</v>
+      </c>
+      <c r="C21" s="1">
+        <v>45767</v>
       </c>
       <c r="D21" s="1">
-        <v>44895</v>
+        <v>45091</v>
       </c>
       <c r="E21" s="1">
-        <v>45406</v>
+        <v>45767</v>
       </c>
       <c r="F21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J21">
-        <v>606</v>
+        <v>639</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A22">
-        <v>639</v>
+        <v>644</v>
       </c>
       <c r="B22" s="1">
-        <v>45089</v>
+        <v>45008</v>
       </c>
       <c r="C22" s="1">
-        <v>45767</v>
+        <v>45699</v>
       </c>
       <c r="D22" s="1">
-        <v>45091</v>
+        <v>45008</v>
       </c>
       <c r="E22" s="1">
-        <v>45767</v>
+        <v>45362</v>
       </c>
       <c r="F22">
         <v>0</v>
-      </c>
-      <c r="J22">
-        <v>639</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A23">
-        <v>644</v>
+        <v>716</v>
       </c>
       <c r="B23" s="1">
-        <v>45008</v>
-      </c>
-      <c r="C23" s="1">
-        <v>45699</v>
+        <v>44562</v>
       </c>
       <c r="D23" s="1">
-        <v>45008</v>
-      </c>
-      <c r="E23" s="1">
-        <v>45362</v>
+        <v>44562</v>
       </c>
       <c r="F23">
         <v>0</v>
+      </c>
+      <c r="J23">
+        <v>716</v>
+      </c>
+      <c r="K23" s="3">
+        <v>716</v>
+      </c>
+      <c r="L23" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A24">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="B24" s="1">
-        <v>44562</v>
+        <v>44958</v>
+      </c>
+      <c r="C24" s="1">
+        <v>45247</v>
       </c>
       <c r="D24" s="1">
-        <v>44562</v>
+        <v>44958</v>
+      </c>
+      <c r="E24" s="1">
+        <v>45245</v>
       </c>
       <c r="F24">
         <v>0</v>
-      </c>
-      <c r="J24">
-        <v>716</v>
-      </c>
-      <c r="K24" s="3">
-        <v>716</v>
-      </c>
-      <c r="L24" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A25">
-        <v>717</v>
+        <v>719</v>
       </c>
       <c r="B25" s="1">
-        <v>44958</v>
-      </c>
-      <c r="C25" s="1">
-        <v>45247</v>
+        <v>44562</v>
       </c>
       <c r="D25" s="1">
-        <v>44958</v>
-      </c>
-      <c r="E25" s="1">
-        <v>45245</v>
+        <v>44562</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J25">
         <v>719</v>
@@ -1504,233 +1510,242 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A26">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="B26" s="1">
-        <v>44562</v>
+        <v>44592</v>
+      </c>
+      <c r="C26" s="1">
+        <v>45757</v>
       </c>
       <c r="D26" s="1">
-        <v>44562</v>
+        <v>44592</v>
+      </c>
+      <c r="E26" s="1">
+        <v>45756</v>
       </c>
       <c r="F26">
         <v>1</v>
       </c>
+      <c r="J26">
+        <v>721</v>
+      </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A27">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="B27" s="1">
-        <v>44592</v>
-      </c>
-      <c r="C27" s="1">
-        <v>45757</v>
+        <v>44562</v>
       </c>
       <c r="D27" s="1">
-        <v>44592</v>
-      </c>
-      <c r="E27" s="1">
-        <v>45756</v>
+        <v>44562</v>
       </c>
       <c r="F27">
         <v>1</v>
       </c>
       <c r="J27">
-        <v>721</v>
+        <v>722</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A28">
-        <v>722</v>
+        <v>724</v>
       </c>
       <c r="B28" s="1">
-        <v>44562</v>
+        <v>44598</v>
       </c>
       <c r="D28" s="1">
-        <v>44562</v>
+        <v>44599</v>
       </c>
       <c r="F28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J28">
-        <v>722</v>
+        <v>724</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A29">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="B29" s="1">
-        <v>44598</v>
+        <v>44562</v>
       </c>
       <c r="D29" s="1">
-        <v>44599</v>
+        <v>44563</v>
       </c>
       <c r="F29">
         <v>0</v>
       </c>
       <c r="J29">
-        <v>724</v>
+        <v>725</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A30">
-        <v>725</v>
+        <v>727</v>
       </c>
       <c r="B30" s="1">
-        <v>44562</v>
+        <v>44779</v>
+      </c>
+      <c r="C30" s="1">
+        <v>44966</v>
       </c>
       <c r="D30" s="1">
-        <v>44563</v>
+        <v>44779</v>
+      </c>
+      <c r="E30" s="1">
+        <v>44966</v>
       </c>
       <c r="F30">
         <v>0</v>
-      </c>
-      <c r="J30">
-        <v>725</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A31">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="B31" s="1">
-        <v>44779</v>
+        <v>44562</v>
       </c>
       <c r="C31" s="1">
-        <v>44966</v>
+        <v>45678</v>
       </c>
       <c r="D31" s="1">
-        <v>44779</v>
+        <v>44562</v>
       </c>
       <c r="E31" s="1">
-        <v>44966</v>
+        <v>45678</v>
       </c>
       <c r="F31">
         <v>0</v>
+      </c>
+      <c r="J31">
+        <v>728</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A32">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="B32" s="1">
         <v>44562</v>
       </c>
       <c r="C32" s="1">
-        <v>45678</v>
+        <v>45292</v>
       </c>
       <c r="D32" s="1">
         <v>44562</v>
       </c>
       <c r="E32" s="1">
-        <v>45678</v>
+        <v>45292</v>
       </c>
       <c r="F32">
         <v>0</v>
       </c>
       <c r="J32">
-        <v>728</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.45">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A33">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="B33" s="1">
-        <v>44562</v>
+        <v>44641</v>
       </c>
       <c r="C33" s="1">
-        <v>45292</v>
+        <v>45893</v>
       </c>
       <c r="D33" s="1">
-        <v>44562</v>
+        <v>44940</v>
       </c>
       <c r="E33" s="1">
-        <v>45292</v>
+        <v>45893</v>
       </c>
       <c r="F33">
         <v>0</v>
       </c>
       <c r="J33">
-        <v>729</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.45">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A34">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="B34" s="1">
-        <v>44641</v>
-      </c>
-      <c r="C34" s="1">
-        <v>45893</v>
+        <v>44936</v>
       </c>
       <c r="D34" s="1">
-        <v>44940</v>
-      </c>
-      <c r="E34" s="1">
-        <v>44941</v>
+        <v>44936</v>
       </c>
       <c r="F34">
         <v>0</v>
       </c>
       <c r="J34">
-        <v>730</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.45">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A35">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="B35" s="1">
-        <v>44936</v>
+        <v>44944</v>
+      </c>
+      <c r="C35" s="1">
+        <v>45019</v>
       </c>
       <c r="D35" s="1">
-        <v>44936</v>
+        <v>45019</v>
+      </c>
+      <c r="E35" s="1">
+        <v>45019</v>
       </c>
       <c r="F35">
         <v>0</v>
       </c>
       <c r="J35">
-        <v>731</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.45">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A36">
-        <v>732</v>
+        <v>734</v>
       </c>
       <c r="B36" s="1">
-        <v>44944</v>
+        <v>45060</v>
       </c>
       <c r="C36" s="1">
-        <v>45019</v>
+        <v>45747</v>
       </c>
       <c r="D36" s="1">
-        <v>45019</v>
+        <v>45060</v>
       </c>
       <c r="E36" s="1">
-        <v>45019</v>
+        <v>45747</v>
       </c>
       <c r="F36">
         <v>0</v>
       </c>
       <c r="J36">
-        <v>732</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.45">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A37">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="B37" s="1">
-        <v>45060</v>
+        <v>45035</v>
       </c>
       <c r="C37" s="1">
         <v>45747</v>
       </c>
       <c r="D37" s="1">
-        <v>45060</v>
+        <v>45035</v>
       </c>
       <c r="E37" s="1">
         <v>45747</v>
@@ -1742,167 +1757,176 @@
         <v>734</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A38">
+        <v>736</v>
+      </c>
+      <c r="B38" s="1">
+        <v>45039</v>
+      </c>
+      <c r="C38" s="1">
+        <v>45050</v>
+      </c>
+      <c r="D38" s="1">
+        <v>45039</v>
+      </c>
+      <c r="E38" s="1">
+        <v>45050</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="J38">
         <v>735</v>
       </c>
-      <c r="B38" s="1">
-        <v>45035</v>
-      </c>
-      <c r="C38" s="1">
-        <v>45747</v>
-      </c>
-      <c r="D38" s="1">
-        <v>45035</v>
-      </c>
-      <c r="E38" s="1">
-        <v>45747</v>
-      </c>
-      <c r="F38">
-        <v>0</v>
-      </c>
-      <c r="J38">
-        <v>734</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A39">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="B39" s="1">
-        <v>45039</v>
+        <v>45704</v>
       </c>
       <c r="C39" s="1">
-        <v>45050</v>
+        <v>45749</v>
       </c>
       <c r="D39" s="1">
-        <v>45039</v>
+        <v>45704</v>
       </c>
       <c r="E39" s="1">
-        <v>45050</v>
+        <v>45749</v>
       </c>
       <c r="F39">
         <v>0</v>
       </c>
       <c r="J39">
-        <v>735</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.45">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A40">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="B40" s="1">
-        <v>45704</v>
+        <v>44584</v>
       </c>
       <c r="C40" s="1">
-        <v>45749</v>
+        <v>45614</v>
       </c>
       <c r="D40" s="1">
-        <v>45704</v>
+        <v>44584</v>
       </c>
       <c r="E40" s="1">
-        <v>45749</v>
+        <v>45614</v>
       </c>
       <c r="F40">
         <v>0</v>
       </c>
       <c r="J40">
-        <v>738</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.45">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A41">
-        <v>739</v>
+        <v>742</v>
       </c>
       <c r="B41" s="1">
-        <v>44584</v>
+        <v>44562</v>
       </c>
       <c r="C41" s="1">
-        <v>45614</v>
+        <v>45520</v>
       </c>
       <c r="D41" s="1">
-        <v>44584</v>
+        <v>44562</v>
       </c>
       <c r="E41" s="1">
-        <v>45614</v>
+        <v>45520</v>
       </c>
       <c r="F41">
         <v>0</v>
       </c>
       <c r="J41">
-        <v>739</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.45">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A42">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="B42" s="1">
-        <v>44562</v>
+        <v>44585</v>
       </c>
       <c r="C42" s="1">
-        <v>45520</v>
+        <v>45687</v>
       </c>
       <c r="D42" s="1">
-        <v>44562</v>
+        <v>44585</v>
       </c>
       <c r="E42" s="1">
-        <v>45520</v>
+        <v>45253</v>
       </c>
       <c r="F42">
         <v>0</v>
       </c>
-      <c r="J42">
-        <v>742</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A43">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="B43" s="1">
-        <v>44585</v>
-      </c>
-      <c r="C43" s="1">
-        <v>45687</v>
+        <v>44600</v>
       </c>
       <c r="D43" s="1">
-        <v>44585</v>
+        <v>44601</v>
       </c>
       <c r="E43" s="1">
-        <v>45253</v>
+        <v>45897</v>
       </c>
       <c r="F43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="J43">
+        <v>744</v>
+      </c>
+      <c r="K43" s="2">
+        <v>745</v>
+      </c>
+      <c r="L43" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A44">
-        <v>744</v>
+        <v>747</v>
       </c>
       <c r="B44" s="1">
-        <v>44600</v>
+        <v>44562</v>
       </c>
       <c r="D44" s="1">
-        <v>44601</v>
+        <v>44562</v>
       </c>
       <c r="F44">
         <v>0</v>
       </c>
       <c r="J44">
-        <v>744</v>
+        <v>747</v>
       </c>
       <c r="K44" s="2">
-        <v>745</v>
+        <v>748</v>
       </c>
       <c r="L44" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+      <c r="M44" s="2">
+        <v>762</v>
+      </c>
+      <c r="N44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A45">
-        <v>747</v>
+        <v>763</v>
       </c>
       <c r="B45" s="1">
         <v>44562</v>
@@ -1914,133 +1938,136 @@
         <v>0</v>
       </c>
       <c r="J45">
-        <v>747</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.45">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A46">
-        <v>762</v>
+        <v>765</v>
       </c>
       <c r="B46" s="1">
-        <v>44910</v>
+        <v>44562</v>
+      </c>
+      <c r="C46" s="1">
+        <v>45785</v>
       </c>
       <c r="D46" s="1">
-        <v>44910</v>
+        <v>44562</v>
+      </c>
+      <c r="E46" s="1">
+        <v>45785</v>
       </c>
       <c r="F46">
         <v>1</v>
       </c>
       <c r="J46">
-        <v>762</v>
-      </c>
-      <c r="K46" s="2">
-        <v>748</v>
-      </c>
-      <c r="L46" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.45">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A47">
-        <v>763</v>
+        <v>766</v>
       </c>
       <c r="B47" s="1">
-        <v>44562</v>
+        <v>44585</v>
+      </c>
+      <c r="C47" s="1">
+        <v>44592</v>
       </c>
       <c r="D47" s="1">
-        <v>44562</v>
+        <v>44585</v>
+      </c>
+      <c r="E47" s="1">
+        <v>44592</v>
       </c>
       <c r="F47">
         <v>0</v>
       </c>
       <c r="J47">
-        <v>763</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.45">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A48">
-        <v>765</v>
+        <v>767</v>
       </c>
       <c r="B48" s="1">
         <v>44562</v>
       </c>
       <c r="C48" s="1">
-        <v>45785</v>
+        <v>45488</v>
       </c>
       <c r="D48" s="1">
         <v>44562</v>
       </c>
       <c r="E48" s="1">
-        <v>45785</v>
+        <v>45488</v>
       </c>
       <c r="F48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J48">
-        <v>765</v>
+        <v>767</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A49">
-        <v>766</v>
+        <v>768</v>
       </c>
       <c r="B49" s="1">
-        <v>44585</v>
+        <v>44604</v>
       </c>
       <c r="C49" s="1">
-        <v>44592</v>
+        <v>44636</v>
       </c>
       <c r="D49" s="1">
-        <v>44585</v>
+        <v>44604</v>
       </c>
       <c r="E49" s="1">
-        <v>44592</v>
+        <v>44636</v>
       </c>
       <c r="F49">
         <v>0</v>
-      </c>
-      <c r="J49">
-        <v>766</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A50">
-        <v>767</v>
+        <v>769</v>
       </c>
       <c r="B50" s="1">
-        <v>44562</v>
+        <v>44603</v>
       </c>
       <c r="C50" s="1">
-        <v>45488</v>
+        <v>45605</v>
       </c>
       <c r="D50" s="1">
-        <v>44562</v>
+        <v>44603</v>
       </c>
       <c r="E50" s="1">
-        <v>45488</v>
+        <v>45605</v>
       </c>
       <c r="F50">
         <v>0</v>
       </c>
       <c r="J50">
-        <v>767</v>
+        <v>769</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A51">
-        <v>768</v>
+        <v>770</v>
       </c>
       <c r="B51" s="1">
-        <v>44604</v>
+        <v>44562</v>
       </c>
       <c r="C51" s="1">
-        <v>44636</v>
+        <v>45224</v>
       </c>
       <c r="D51" s="1">
-        <v>44604</v>
+        <v>44563</v>
       </c>
       <c r="E51" s="1">
-        <v>44636</v>
+        <v>45224</v>
       </c>
       <c r="F51">
         <v>0</v>
@@ -2048,62 +2075,56 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A52">
-        <v>769</v>
+        <v>771</v>
       </c>
       <c r="B52" s="1">
-        <v>44603</v>
+        <v>44562</v>
       </c>
       <c r="C52" s="1">
-        <v>45605</v>
+        <v>45666</v>
       </c>
       <c r="D52" s="1">
-        <v>44603</v>
+        <v>44576</v>
       </c>
       <c r="E52" s="1">
-        <v>45605</v>
+        <v>45666</v>
       </c>
       <c r="F52">
         <v>0</v>
-      </c>
-      <c r="J52">
-        <v>769</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A53">
-        <v>770</v>
+        <v>773</v>
       </c>
       <c r="B53" s="1">
-        <v>44562</v>
-      </c>
-      <c r="C53" s="1">
-        <v>45224</v>
+        <v>44586</v>
       </c>
       <c r="D53" s="1">
-        <v>44563</v>
-      </c>
-      <c r="E53" s="1">
-        <v>45224</v>
+        <v>44586</v>
       </c>
       <c r="F53">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="J53">
+        <v>773</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A54">
-        <v>771</v>
+        <v>774</v>
       </c>
       <c r="B54" s="1">
-        <v>44562</v>
+        <v>44586</v>
       </c>
       <c r="C54" s="1">
-        <v>45666</v>
+        <v>45085</v>
       </c>
       <c r="D54" s="1">
-        <v>44576</v>
+        <v>44586</v>
       </c>
       <c r="E54" s="1">
-        <v>45666</v>
+        <v>45083</v>
       </c>
       <c r="F54">
         <v>0</v>
@@ -2111,279 +2132,279 @@
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A55">
-        <v>773</v>
+        <v>775</v>
       </c>
       <c r="B55" s="1">
-        <v>44586</v>
+        <v>44579</v>
       </c>
       <c r="D55" s="1">
-        <v>44586</v>
+        <v>44589</v>
       </c>
       <c r="F55">
         <v>1</v>
       </c>
       <c r="J55">
-        <v>773</v>
+        <v>775</v>
+      </c>
+      <c r="K55" s="2">
+        <v>776</v>
+      </c>
+      <c r="L55" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A56">
-        <v>774</v>
+        <v>777</v>
       </c>
       <c r="B56" s="1">
-        <v>44586</v>
-      </c>
-      <c r="C56" s="1">
-        <v>45085</v>
+        <v>44562</v>
       </c>
       <c r="D56" s="1">
-        <v>44586</v>
+        <v>44562</v>
       </c>
       <c r="E56" s="1">
-        <v>45083</v>
+        <v>45897</v>
       </c>
       <c r="F56">
         <v>0</v>
+      </c>
+      <c r="J56">
+        <v>777</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A57">
-        <v>775</v>
+        <v>778</v>
       </c>
       <c r="B57" s="1">
-        <v>44579</v>
+        <v>44562</v>
       </c>
       <c r="D57" s="1">
-        <v>44589</v>
+        <v>44562</v>
       </c>
       <c r="F57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J57">
-        <v>775</v>
-      </c>
-      <c r="K57" s="2">
-        <v>776</v>
-      </c>
-      <c r="L57" t="s">
-        <v>11</v>
+        <v>778</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A58">
-        <v>777</v>
+        <v>779</v>
       </c>
       <c r="B58" s="1">
-        <v>44562</v>
+        <v>44572</v>
+      </c>
+      <c r="C58" s="1">
+        <v>45239</v>
       </c>
       <c r="D58" s="1">
-        <v>44562</v>
+        <v>44573</v>
+      </c>
+      <c r="E58" s="1">
+        <v>45239</v>
       </c>
       <c r="F58">
         <v>0</v>
       </c>
       <c r="J58">
-        <v>777</v>
+        <v>779</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A59">
-        <v>778</v>
+        <v>781</v>
       </c>
       <c r="B59" s="1">
         <v>44562</v>
       </c>
+      <c r="C59" s="1">
+        <v>45755</v>
+      </c>
       <c r="D59" s="1">
         <v>44562</v>
       </c>
+      <c r="E59" s="1">
+        <v>45748</v>
+      </c>
       <c r="F59">
         <v>0</v>
-      </c>
-      <c r="J59">
-        <v>778</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A60">
-        <v>779</v>
+        <v>782</v>
       </c>
       <c r="B60" s="1">
-        <v>44572</v>
-      </c>
-      <c r="C60" s="1">
-        <v>45239</v>
+        <v>44562</v>
       </c>
       <c r="D60" s="1">
-        <v>44573</v>
-      </c>
-      <c r="E60" s="1">
-        <v>45239</v>
+        <v>44562</v>
       </c>
       <c r="F60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J60">
-        <v>779</v>
+        <v>782</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A61">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="B61" s="1">
         <v>44562</v>
       </c>
       <c r="C61" s="1">
-        <v>45755</v>
+        <v>45747</v>
       </c>
       <c r="D61" s="1">
         <v>44562</v>
       </c>
       <c r="E61" s="1">
-        <v>45748</v>
+        <v>45747</v>
       </c>
       <c r="F61">
         <v>0</v>
+      </c>
+      <c r="J61">
+        <v>783</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A62">
-        <v>782</v>
+        <v>785</v>
       </c>
       <c r="B62" s="1">
         <v>44562</v>
       </c>
+      <c r="C62" s="1">
+        <v>45023</v>
+      </c>
       <c r="D62" s="1">
         <v>44562</v>
       </c>
+      <c r="E62" s="1">
+        <v>45023</v>
+      </c>
       <c r="F62">
-        <v>1</v>
-      </c>
-      <c r="J62">
-        <v>782</v>
+        <v>0</v>
+      </c>
+      <c r="K62" s="2">
+        <v>784</v>
+      </c>
+      <c r="L62" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A63">
-        <v>783</v>
+        <v>786</v>
       </c>
       <c r="B63" s="1">
         <v>44562</v>
       </c>
       <c r="C63" s="1">
-        <v>45747</v>
+        <v>45872</v>
       </c>
       <c r="D63" s="1">
-        <v>44562</v>
+        <v>44563</v>
       </c>
       <c r="E63" s="1">
-        <v>45747</v>
+        <v>45872</v>
       </c>
       <c r="F63">
         <v>0</v>
       </c>
       <c r="J63">
-        <v>783</v>
+        <v>786</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A64">
-        <v>785</v>
+        <v>787</v>
       </c>
       <c r="B64" s="1">
-        <v>44562</v>
+        <v>44573</v>
       </c>
       <c r="C64" s="1">
-        <v>45023</v>
+        <v>45543</v>
       </c>
       <c r="D64" s="1">
-        <v>44562</v>
+        <v>44573</v>
       </c>
       <c r="E64" s="1">
-        <v>45023</v>
+        <v>45543</v>
       </c>
       <c r="F64">
-        <v>0</v>
-      </c>
-      <c r="K64" s="2">
-        <v>784</v>
-      </c>
-      <c r="L64" t="s">
-        <v>12</v>
+        <v>1</v>
+      </c>
+      <c r="J64">
+        <v>787</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A65">
-        <v>786</v>
+        <v>789</v>
       </c>
       <c r="B65" s="1">
-        <v>44562</v>
-      </c>
-      <c r="C65" s="1">
-        <v>45872</v>
+        <v>44574</v>
       </c>
       <c r="D65" s="1">
-        <v>44563</v>
-      </c>
-      <c r="E65" s="1">
-        <v>45872</v>
+        <v>44574</v>
       </c>
       <c r="F65">
         <v>0</v>
       </c>
       <c r="J65">
-        <v>786</v>
+        <v>789</v>
+      </c>
+      <c r="K65" s="2">
+        <v>788</v>
+      </c>
+      <c r="L65" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A66">
-        <v>787</v>
+        <v>790</v>
       </c>
       <c r="B66" s="1">
-        <v>44573</v>
-      </c>
-      <c r="C66" s="1">
-        <v>45543</v>
+        <v>44562</v>
       </c>
       <c r="D66" s="1">
-        <v>44573</v>
-      </c>
-      <c r="E66" s="1">
-        <v>45543</v>
+        <v>44562</v>
       </c>
       <c r="F66">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J66">
-        <v>787</v>
+        <v>790</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A67">
-        <v>789</v>
+        <v>791</v>
       </c>
       <c r="B67" s="1">
-        <v>44574</v>
+        <v>44562</v>
       </c>
       <c r="D67" s="1">
-        <v>44574</v>
+        <v>44578</v>
       </c>
       <c r="F67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J67">
-        <v>789</v>
-      </c>
-      <c r="K67" s="2">
-        <v>788</v>
-      </c>
-      <c r="L67" t="s">
-        <v>8</v>
+        <v>791</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A68">
-        <v>790</v>
+        <v>792</v>
       </c>
       <c r="B68" s="1">
         <v>44562</v>
@@ -2395,1151 +2416,1107 @@
         <v>0</v>
       </c>
       <c r="J68">
-        <v>790</v>
+        <v>792</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A69">
-        <v>791</v>
+        <v>793</v>
       </c>
       <c r="B69" s="1">
         <v>44562</v>
       </c>
+      <c r="C69" s="1">
+        <v>45793</v>
+      </c>
       <c r="D69" s="1">
-        <v>44578</v>
+        <v>44562</v>
+      </c>
+      <c r="E69" s="1">
+        <v>45793</v>
       </c>
       <c r="F69">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J69">
-        <v>791</v>
+        <v>793</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A70">
-        <v>792</v>
+        <v>794</v>
       </c>
       <c r="B70" s="1">
         <v>44562</v>
       </c>
+      <c r="C70" s="1">
+        <v>45255</v>
+      </c>
       <c r="D70" s="1">
         <v>44562</v>
       </c>
+      <c r="E70" s="1">
+        <v>45255</v>
+      </c>
       <c r="F70">
         <v>0</v>
       </c>
       <c r="J70">
-        <v>792</v>
+        <v>794</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A71">
-        <v>793</v>
+        <v>796</v>
       </c>
       <c r="B71" s="1">
-        <v>44562</v>
+        <v>44568</v>
       </c>
       <c r="C71" s="1">
-        <v>45793</v>
+        <v>44774</v>
       </c>
       <c r="D71" s="1">
-        <v>44562</v>
+        <v>44570</v>
       </c>
       <c r="E71" s="1">
-        <v>45793</v>
+        <v>44772</v>
       </c>
       <c r="F71">
         <v>0</v>
       </c>
       <c r="J71">
-        <v>793</v>
+        <v>796</v>
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A72">
-        <v>794</v>
+        <v>832</v>
       </c>
       <c r="B72" s="1">
         <v>44562</v>
       </c>
       <c r="C72" s="1">
-        <v>45255</v>
+        <v>45785</v>
       </c>
       <c r="D72" s="1">
         <v>44562</v>
       </c>
       <c r="E72" s="1">
-        <v>45255</v>
+        <v>45785</v>
       </c>
       <c r="F72">
         <v>0</v>
       </c>
       <c r="J72">
-        <v>794</v>
+        <v>832</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A73">
-        <v>796</v>
+        <v>833</v>
       </c>
       <c r="B73" s="1">
-        <v>44568</v>
+        <v>44562</v>
       </c>
       <c r="C73" s="1">
-        <v>44774</v>
+        <v>45097</v>
       </c>
       <c r="D73" s="1">
-        <v>44570</v>
+        <v>44562</v>
       </c>
       <c r="E73" s="1">
-        <v>44772</v>
+        <v>45097</v>
       </c>
       <c r="F73">
         <v>0</v>
       </c>
       <c r="J73">
-        <v>796</v>
+        <v>833</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A74">
-        <v>832</v>
+        <v>834</v>
       </c>
       <c r="B74" s="1">
         <v>44562</v>
       </c>
-      <c r="C74" s="1">
-        <v>45785</v>
-      </c>
       <c r="D74" s="1">
         <v>44562</v>
       </c>
-      <c r="E74" s="1">
-        <v>45785</v>
-      </c>
       <c r="F74">
         <v>0</v>
       </c>
       <c r="J74">
-        <v>832</v>
+        <v>834</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A75">
-        <v>833</v>
+        <v>835</v>
       </c>
       <c r="B75" s="1">
-        <v>44562</v>
+        <v>44572</v>
       </c>
       <c r="C75" s="1">
-        <v>45097</v>
+        <v>45845</v>
       </c>
       <c r="D75" s="1">
-        <v>44562</v>
+        <v>44572</v>
       </c>
       <c r="E75" s="1">
-        <v>45097</v>
+        <v>45761</v>
       </c>
       <c r="F75">
         <v>0</v>
-      </c>
-      <c r="J75">
-        <v>833</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A76">
-        <v>834</v>
+        <v>836</v>
       </c>
       <c r="B76" s="1">
-        <v>44562</v>
+        <v>45543</v>
+      </c>
+      <c r="C76" s="1">
+        <v>45845</v>
       </c>
       <c r="D76" s="1">
-        <v>44562</v>
+        <v>45543</v>
+      </c>
+      <c r="E76" s="1">
+        <v>45748</v>
       </c>
       <c r="F76">
         <v>0</v>
       </c>
       <c r="J76">
-        <v>834</v>
+        <v>836</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A77">
-        <v>835</v>
+        <v>837</v>
       </c>
       <c r="B77" s="1">
-        <v>44572</v>
-      </c>
-      <c r="C77" s="1">
-        <v>45845</v>
+        <v>44849</v>
       </c>
       <c r="D77" s="1">
-        <v>44572</v>
-      </c>
-      <c r="E77" s="1">
-        <v>45761</v>
+        <v>44849</v>
       </c>
       <c r="F77">
         <v>0</v>
+      </c>
+      <c r="J77">
+        <v>837</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A78">
-        <v>836</v>
+        <v>838</v>
       </c>
       <c r="B78" s="1">
-        <v>45543</v>
-      </c>
-      <c r="C78" s="1">
-        <v>45845</v>
+        <v>45207</v>
       </c>
       <c r="D78" s="1">
-        <v>45543</v>
-      </c>
-      <c r="E78" s="1">
-        <v>45748</v>
+        <v>45207</v>
       </c>
       <c r="F78">
         <v>0</v>
       </c>
       <c r="J78">
-        <v>836</v>
+        <v>838</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A79">
-        <v>837</v>
+        <v>839</v>
       </c>
       <c r="B79" s="1">
-        <v>44849</v>
+        <v>44562</v>
+      </c>
+      <c r="C79" s="1">
+        <v>44939</v>
       </c>
       <c r="D79" s="1">
-        <v>44849</v>
+        <v>44562</v>
+      </c>
+      <c r="E79" s="1">
+        <v>44829</v>
       </c>
       <c r="F79">
         <v>0</v>
-      </c>
-      <c r="J79">
-        <v>837</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A80">
-        <v>838</v>
+        <v>840</v>
       </c>
       <c r="B80" s="1">
-        <v>45207</v>
+        <v>44568</v>
       </c>
       <c r="D80" s="1">
-        <v>45207</v>
+        <v>44568</v>
       </c>
       <c r="F80">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J80">
-        <v>838</v>
+        <v>840</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A81">
-        <v>839</v>
+        <v>841</v>
       </c>
       <c r="B81" s="1">
         <v>44562</v>
       </c>
       <c r="C81" s="1">
-        <v>44939</v>
+        <v>45774</v>
       </c>
       <c r="D81" s="1">
         <v>44562</v>
       </c>
       <c r="E81" s="1">
-        <v>44829</v>
+        <v>45774</v>
       </c>
       <c r="F81">
         <v>0</v>
+      </c>
+      <c r="K81" s="2">
+        <v>842</v>
+      </c>
+      <c r="L81" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A82">
-        <v>840</v>
+        <v>843</v>
       </c>
       <c r="B82" s="1">
-        <v>44568</v>
+        <v>44562</v>
+      </c>
+      <c r="C82" s="1">
+        <v>45731</v>
       </c>
       <c r="D82" s="1">
-        <v>44568</v>
+        <v>44800</v>
+      </c>
+      <c r="E82" s="1">
+        <v>45731</v>
       </c>
       <c r="F82">
         <v>1</v>
       </c>
       <c r="J82">
-        <v>840</v>
+        <v>843</v>
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A83">
-        <v>841</v>
+        <v>864</v>
       </c>
       <c r="B83" s="1">
         <v>44562</v>
       </c>
       <c r="C83" s="1">
-        <v>45774</v>
+        <v>45426</v>
       </c>
       <c r="D83" s="1">
         <v>44562</v>
       </c>
       <c r="E83" s="1">
-        <v>45774</v>
+        <v>45426</v>
       </c>
       <c r="F83">
         <v>0</v>
+      </c>
+      <c r="J83">
+        <v>864</v>
       </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A84">
-        <v>843</v>
+        <v>865</v>
       </c>
       <c r="B84" s="1">
-        <v>44562</v>
+        <v>44611</v>
       </c>
       <c r="C84" s="1">
-        <v>45731</v>
+        <v>44905</v>
       </c>
       <c r="D84" s="1">
-        <v>44800</v>
+        <v>44611</v>
       </c>
       <c r="E84" s="1">
-        <v>45731</v>
+        <v>44905</v>
       </c>
       <c r="F84">
-        <v>1</v>
-      </c>
-      <c r="K84" s="2">
-        <v>842</v>
-      </c>
-      <c r="L84" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A85">
-        <v>864</v>
+        <v>866</v>
       </c>
       <c r="B85" s="1">
         <v>44562</v>
       </c>
-      <c r="C85" s="1">
-        <v>45426</v>
-      </c>
       <c r="D85" s="1">
         <v>44562</v>
       </c>
-      <c r="E85" s="1">
-        <v>45426</v>
-      </c>
       <c r="F85">
         <v>0</v>
       </c>
       <c r="J85">
-        <v>843</v>
+        <v>866</v>
       </c>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A86">
-        <v>865</v>
+        <v>867</v>
       </c>
       <c r="B86" s="1">
-        <v>44611</v>
+        <v>44576</v>
       </c>
       <c r="C86" s="1">
-        <v>44905</v>
+        <v>45106</v>
       </c>
       <c r="D86" s="1">
-        <v>44611</v>
+        <v>44576</v>
       </c>
       <c r="E86" s="1">
-        <v>44905</v>
+        <v>45106</v>
       </c>
       <c r="F86">
         <v>0</v>
       </c>
       <c r="J86">
-        <v>864</v>
+        <v>867</v>
       </c>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A87">
-        <v>866</v>
+        <v>868</v>
       </c>
       <c r="B87" s="1">
         <v>44562</v>
       </c>
+      <c r="C87" s="1">
+        <v>45206</v>
+      </c>
       <c r="D87" s="1">
         <v>44562</v>
       </c>
+      <c r="E87" s="1">
+        <v>45206</v>
+      </c>
       <c r="F87">
         <v>0</v>
       </c>
       <c r="J87">
-        <v>866</v>
+        <v>868</v>
       </c>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A88">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="B88" s="1">
-        <v>44576</v>
+        <v>44562</v>
       </c>
       <c r="C88" s="1">
-        <v>45106</v>
+        <v>45215</v>
       </c>
       <c r="D88" s="1">
-        <v>44576</v>
+        <v>44562</v>
       </c>
       <c r="E88" s="1">
-        <v>45106</v>
+        <v>45210</v>
       </c>
       <c r="F88">
         <v>0</v>
-      </c>
-      <c r="J88">
-        <v>867</v>
       </c>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A89">
-        <v>868</v>
+        <v>870</v>
       </c>
       <c r="B89" s="1">
         <v>44562</v>
       </c>
-      <c r="C89" s="1">
-        <v>45206</v>
-      </c>
       <c r="D89" s="1">
         <v>44562</v>
       </c>
-      <c r="E89" s="1">
-        <v>45206</v>
-      </c>
       <c r="F89">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J89">
-        <v>868</v>
+        <v>870</v>
       </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A90">
-        <v>869</v>
+        <v>871</v>
       </c>
       <c r="B90" s="1">
         <v>44562</v>
       </c>
-      <c r="C90" s="1">
-        <v>45215</v>
-      </c>
       <c r="D90" s="1">
         <v>44562</v>
       </c>
-      <c r="E90" s="1">
-        <v>45210</v>
-      </c>
       <c r="F90">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="J90">
+        <v>871</v>
       </c>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A91">
-        <v>870</v>
+        <v>873</v>
       </c>
       <c r="B91" s="1">
-        <v>44562</v>
+        <v>44697</v>
       </c>
       <c r="D91" s="1">
-        <v>44562</v>
+        <v>44698</v>
+      </c>
+      <c r="E91" s="1">
+        <v>44982</v>
       </c>
       <c r="F91">
-        <v>1</v>
-      </c>
-      <c r="J91">
-        <v>870</v>
+        <v>0</v>
+      </c>
+      <c r="K91" s="2">
+        <v>872</v>
+      </c>
+      <c r="L91" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A92">
-        <v>871</v>
+        <v>875</v>
       </c>
       <c r="B92" s="1">
         <v>44562</v>
       </c>
+      <c r="C92" s="1">
+        <v>45181</v>
+      </c>
       <c r="D92" s="1">
         <v>44562</v>
       </c>
+      <c r="E92" s="1">
+        <v>45181</v>
+      </c>
       <c r="F92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J92">
-        <v>871</v>
+        <v>875</v>
+      </c>
+      <c r="K92" s="2">
+        <v>874</v>
+      </c>
+      <c r="L92" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A93">
-        <v>873</v>
+        <v>876</v>
       </c>
       <c r="B93" s="1">
-        <v>44697</v>
+        <v>44837</v>
       </c>
       <c r="D93" s="1">
-        <v>44698</v>
+        <v>44838</v>
       </c>
       <c r="F93">
         <v>0</v>
       </c>
-      <c r="K93" s="2">
-        <v>872</v>
-      </c>
-      <c r="L93" t="s">
-        <v>13</v>
+      <c r="J93">
+        <v>876</v>
       </c>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A94">
-        <v>875</v>
+        <v>877</v>
       </c>
       <c r="B94" s="1">
-        <v>44562</v>
+        <v>44859</v>
       </c>
       <c r="C94" s="1">
-        <v>45181</v>
+        <v>45397</v>
       </c>
       <c r="D94" s="1">
-        <v>44562</v>
+        <v>44859</v>
       </c>
       <c r="E94" s="1">
-        <v>45181</v>
+        <v>45397</v>
       </c>
       <c r="F94">
         <v>0</v>
       </c>
       <c r="J94">
-        <v>875</v>
-      </c>
-      <c r="K94" s="2">
-        <v>874</v>
-      </c>
-      <c r="L94" t="s">
-        <v>8</v>
+        <v>877</v>
       </c>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A95">
-        <v>876</v>
+        <v>878</v>
       </c>
       <c r="B95" s="1">
-        <v>44837</v>
+        <v>44854</v>
+      </c>
+      <c r="C95" s="1">
+        <v>45693</v>
       </c>
       <c r="D95" s="1">
-        <v>44838</v>
+        <v>44854</v>
+      </c>
+      <c r="E95" s="1">
+        <v>45686</v>
       </c>
       <c r="F95">
         <v>0</v>
       </c>
-      <c r="J95">
-        <v>876</v>
+      <c r="K95" s="2">
+        <v>879</v>
+      </c>
+      <c r="L95" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A96">
-        <v>877</v>
+        <v>880</v>
       </c>
       <c r="B96" s="1">
-        <v>44859</v>
+        <v>44562</v>
       </c>
       <c r="C96" s="1">
-        <v>45397</v>
+        <v>44813</v>
       </c>
       <c r="D96" s="1">
-        <v>44859</v>
+        <v>44563</v>
       </c>
       <c r="E96" s="1">
-        <v>45397</v>
+        <v>44676</v>
       </c>
       <c r="F96">
         <v>0</v>
-      </c>
-      <c r="J96">
-        <v>877</v>
       </c>
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A97">
-        <v>878</v>
+        <v>881</v>
       </c>
       <c r="B97" s="1">
-        <v>44854</v>
+        <v>44834</v>
       </c>
       <c r="C97" s="1">
-        <v>45693</v>
+        <v>45287</v>
       </c>
       <c r="D97" s="1">
-        <v>44854</v>
+        <v>44834</v>
       </c>
       <c r="E97" s="1">
-        <v>45686</v>
+        <v>45285</v>
       </c>
       <c r="F97">
         <v>0</v>
-      </c>
-      <c r="K97" s="2">
-        <v>879</v>
-      </c>
-      <c r="L97" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A98">
-        <v>880</v>
+        <v>882</v>
       </c>
       <c r="B98" s="1">
-        <v>44562</v>
-      </c>
-      <c r="C98" s="1">
-        <v>44813</v>
+        <v>44697</v>
       </c>
       <c r="D98" s="1">
-        <v>44563</v>
-      </c>
-      <c r="E98" s="1">
-        <v>44676</v>
+        <v>44698</v>
       </c>
       <c r="F98">
         <v>0</v>
+      </c>
+      <c r="J98">
+        <v>882</v>
       </c>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A99">
-        <v>881</v>
+        <v>883</v>
       </c>
       <c r="B99" s="1">
-        <v>44834</v>
+        <v>44697</v>
       </c>
       <c r="C99" s="1">
-        <v>45287</v>
+        <v>45102</v>
       </c>
       <c r="D99" s="1">
-        <v>44834</v>
+        <v>44698</v>
       </c>
       <c r="E99" s="1">
-        <v>45285</v>
+        <v>45102</v>
       </c>
       <c r="F99">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A100">
-        <v>882</v>
+        <v>935</v>
       </c>
       <c r="B100" s="1">
-        <v>44697</v>
+        <v>44928</v>
       </c>
       <c r="D100" s="1">
-        <v>44698</v>
+        <v>44928</v>
       </c>
       <c r="F100">
         <v>0</v>
       </c>
       <c r="J100">
-        <v>882</v>
+        <v>935</v>
       </c>
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A101">
-        <v>883</v>
+        <v>936</v>
       </c>
       <c r="B101" s="1">
-        <v>44697</v>
+        <v>44948</v>
       </c>
       <c r="C101" s="1">
-        <v>45102</v>
+        <v>45134</v>
       </c>
       <c r="D101" s="1">
-        <v>44698</v>
+        <v>44948</v>
       </c>
       <c r="E101" s="1">
-        <v>45102</v>
+        <v>45134</v>
       </c>
       <c r="F101">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="J101">
+        <v>935</v>
       </c>
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A102">
-        <v>935</v>
+        <v>949</v>
       </c>
       <c r="B102" s="1">
-        <v>44928</v>
+        <v>44844</v>
+      </c>
+      <c r="C102" s="1">
+        <v>45281</v>
       </c>
       <c r="D102" s="1">
-        <v>44928</v>
+        <v>44844</v>
+      </c>
+      <c r="E102" s="1">
+        <v>45281</v>
       </c>
       <c r="F102">
         <v>0</v>
       </c>
       <c r="J102">
-        <v>935</v>
+        <v>936</v>
+      </c>
+      <c r="K102" s="2">
+        <v>937</v>
+      </c>
+      <c r="L102" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A103">
-        <v>936</v>
+        <v>951</v>
       </c>
       <c r="B103" s="1">
-        <v>44948</v>
+        <v>45012</v>
       </c>
       <c r="C103" s="1">
-        <v>45134</v>
+        <v>45785</v>
       </c>
       <c r="D103" s="1">
-        <v>44948</v>
+        <v>45013</v>
       </c>
       <c r="E103" s="1">
-        <v>45134</v>
+        <v>45785</v>
       </c>
       <c r="F103">
         <v>0</v>
       </c>
       <c r="J103">
-        <v>935</v>
+        <v>951</v>
+      </c>
+      <c r="K103" s="2">
+        <v>948</v>
+      </c>
+      <c r="L103" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A104">
-        <v>949</v>
+        <v>952</v>
       </c>
       <c r="B104" s="1">
-        <v>44844</v>
-      </c>
-      <c r="C104" s="1">
-        <v>45281</v>
+        <v>44859</v>
       </c>
       <c r="D104" s="1">
-        <v>44844</v>
+        <v>45705</v>
       </c>
       <c r="E104" s="1">
-        <v>45281</v>
+        <v>45894</v>
       </c>
       <c r="F104">
         <v>0</v>
-      </c>
-      <c r="J104">
-        <v>936</v>
-      </c>
-      <c r="K104" s="2">
-        <v>937</v>
-      </c>
-      <c r="L104" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A105">
-        <v>951</v>
+        <v>953</v>
       </c>
       <c r="B105" s="1">
-        <v>45012</v>
+        <v>44915</v>
       </c>
       <c r="C105" s="1">
-        <v>45785</v>
+        <v>45175</v>
       </c>
       <c r="D105" s="1">
-        <v>45013</v>
+        <v>44955</v>
       </c>
       <c r="E105" s="1">
-        <v>45785</v>
+        <v>45175</v>
       </c>
       <c r="F105">
         <v>0</v>
       </c>
       <c r="J105">
-        <v>951</v>
-      </c>
-      <c r="K105" s="2">
-        <v>948</v>
-      </c>
-      <c r="L105" t="s">
-        <v>8</v>
+        <v>953</v>
       </c>
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A106">
-        <v>952</v>
+        <v>954</v>
       </c>
       <c r="B106" s="1">
-        <v>44859</v>
+        <v>44949</v>
+      </c>
+      <c r="C106" s="1">
+        <v>45369</v>
       </c>
       <c r="D106" s="1">
-        <v>45705</v>
+        <v>45228</v>
+      </c>
+      <c r="E106" s="1">
+        <v>45369</v>
       </c>
       <c r="F106">
         <v>0</v>
+      </c>
+      <c r="J106">
+        <v>954</v>
       </c>
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A107">
-        <v>953</v>
+        <v>955</v>
       </c>
       <c r="B107" s="1">
-        <v>44915</v>
+        <v>44914</v>
       </c>
       <c r="C107" s="1">
-        <v>45175</v>
+        <v>45844</v>
       </c>
       <c r="D107" s="1">
-        <v>44955</v>
+        <v>44976</v>
       </c>
       <c r="E107" s="1">
-        <v>45175</v>
+        <v>45844</v>
       </c>
       <c r="F107">
         <v>0</v>
       </c>
       <c r="J107">
-        <v>953</v>
+        <v>955</v>
       </c>
     </row>
     <row r="108" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A108">
-        <v>954</v>
+        <v>956</v>
       </c>
       <c r="B108" s="1">
-        <v>44949</v>
+        <v>44893</v>
       </c>
       <c r="C108" s="1">
-        <v>45369</v>
+        <v>45675</v>
       </c>
       <c r="D108" s="1">
-        <v>45228</v>
+        <v>44958</v>
       </c>
       <c r="E108" s="1">
-        <v>45369</v>
+        <v>45675</v>
       </c>
       <c r="F108">
         <v>0</v>
       </c>
       <c r="J108">
-        <v>954</v>
+        <v>956</v>
       </c>
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A109">
-        <v>955</v>
+        <v>957</v>
       </c>
       <c r="B109" s="1">
-        <v>44914</v>
+        <v>44893</v>
       </c>
       <c r="C109" s="1">
-        <v>45844</v>
+        <v>45747</v>
       </c>
       <c r="D109" s="1">
-        <v>44976</v>
+        <v>44895</v>
       </c>
       <c r="E109" s="1">
-        <v>45844</v>
+        <v>45747</v>
       </c>
       <c r="F109">
         <v>0</v>
       </c>
       <c r="J109">
-        <v>955</v>
+        <v>957</v>
       </c>
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A110">
-        <v>956</v>
+        <v>998</v>
       </c>
       <c r="B110" s="1">
-        <v>44893</v>
-      </c>
-      <c r="C110" s="1">
-        <v>45675</v>
+        <v>45749</v>
       </c>
       <c r="D110" s="1">
-        <v>44958</v>
-      </c>
-      <c r="E110" s="1">
-        <v>45675</v>
+        <v>45750</v>
       </c>
       <c r="F110">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J110">
-        <v>956</v>
+        <v>998</v>
+      </c>
+      <c r="K110" s="2">
+        <v>997</v>
+      </c>
+      <c r="L110" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="111" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A111">
-        <v>957</v>
+        <v>1000</v>
       </c>
       <c r="B111" s="1">
-        <v>44893</v>
-      </c>
-      <c r="C111" s="1">
-        <v>45747</v>
+        <v>45418</v>
       </c>
       <c r="D111" s="1">
-        <v>44895</v>
-      </c>
-      <c r="E111" s="1">
-        <v>45747</v>
+        <v>45418</v>
       </c>
       <c r="F111">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J111">
-        <v>957</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="112" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A112">
-        <v>998</v>
+        <v>1001</v>
       </c>
       <c r="B112" s="1">
-        <v>45749</v>
+        <v>45483</v>
       </c>
       <c r="D112" s="1">
-        <v>45750</v>
+        <v>45483</v>
       </c>
       <c r="F112">
+        <v>0</v>
+      </c>
+      <c r="J112">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="113" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A113">
+        <v>1024</v>
+      </c>
+      <c r="B113" s="1">
+        <v>45529</v>
+      </c>
+      <c r="C113" s="1">
+        <v>45747</v>
+      </c>
+      <c r="D113" s="1">
+        <v>45529</v>
+      </c>
+      <c r="E113" s="1">
+        <v>45747</v>
+      </c>
+      <c r="F113">
+        <v>0</v>
+      </c>
+      <c r="J113">
+        <v>1024</v>
+      </c>
+      <c r="K113" s="2">
+        <v>1022</v>
+      </c>
+      <c r="L113" t="s">
+        <v>14</v>
+      </c>
+      <c r="M113" s="2">
+        <v>1025</v>
+      </c>
+      <c r="N113" t="s">
+        <v>16</v>
+      </c>
+      <c r="O113" s="2">
+        <v>1026</v>
+      </c>
+      <c r="P113" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="114" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A114">
+        <v>1071</v>
+      </c>
+      <c r="B114" s="1">
+        <v>45731</v>
+      </c>
+      <c r="D114" s="1">
+        <v>45731</v>
+      </c>
+      <c r="E114" s="1">
+        <v>45866</v>
+      </c>
+      <c r="F114">
         <v>1</v>
       </c>
-      <c r="J112">
-        <v>998</v>
-      </c>
-      <c r="K112" s="2">
-        <v>997</v>
-      </c>
-      <c r="L112" t="s">
+      <c r="J114">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="115" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A115">
+        <v>1073</v>
+      </c>
+      <c r="B115" s="1">
+        <v>45752</v>
+      </c>
+      <c r="C115" s="1">
+        <v>45892</v>
+      </c>
+      <c r="D115" s="1">
+        <v>45752</v>
+      </c>
+      <c r="E115" s="1">
+        <v>45892</v>
+      </c>
+      <c r="F115">
+        <v>1</v>
+      </c>
+      <c r="K115" s="2">
+        <v>1078</v>
+      </c>
+      <c r="L115" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A113">
-        <v>1000</v>
-      </c>
-      <c r="B113" s="1">
-        <v>45418</v>
-      </c>
-      <c r="D113" s="1">
-        <v>45418</v>
-      </c>
-      <c r="F113">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A116">
+        <v>1074</v>
+      </c>
+      <c r="B116" s="1">
+        <v>45762</v>
+      </c>
+      <c r="D116" s="1">
+        <v>45762</v>
+      </c>
+      <c r="F116">
         <v>1</v>
       </c>
-      <c r="J113">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A114">
-        <v>1001</v>
-      </c>
-      <c r="B114" s="1">
-        <v>45483</v>
-      </c>
-      <c r="D114" s="1">
-        <v>45483</v>
-      </c>
-      <c r="F114">
-        <v>0</v>
-      </c>
-      <c r="J114">
-        <v>1001</v>
-      </c>
-    </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A115">
-        <v>1024</v>
-      </c>
-      <c r="B115" s="1">
-        <v>45529</v>
-      </c>
-      <c r="C115" s="1">
-        <v>45747</v>
-      </c>
-      <c r="D115" s="1">
-        <v>45529</v>
-      </c>
-      <c r="E115" s="1">
-        <v>45747</v>
-      </c>
-      <c r="F115">
-        <v>0</v>
-      </c>
-      <c r="J115">
-        <v>1024</v>
-      </c>
-      <c r="K115" s="2">
-        <v>1022</v>
-      </c>
-      <c r="L115" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A116">
-        <v>1025</v>
-      </c>
-      <c r="B116" s="1">
-        <v>45529</v>
-      </c>
-      <c r="D116" s="1">
-        <v>45529</v>
-      </c>
-      <c r="F116">
-        <v>0</v>
-      </c>
-      <c r="J116">
-        <v>1025</v>
-      </c>
-    </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="117" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A117">
-        <v>1026</v>
+        <v>1077</v>
       </c>
       <c r="B117" s="1">
-        <v>45529</v>
+        <v>45864</v>
       </c>
       <c r="D117" s="1">
-        <v>45529</v>
+        <v>45864</v>
+      </c>
+      <c r="E117" s="1">
+        <v>45872</v>
       </c>
       <c r="F117">
         <v>1</v>
       </c>
-      <c r="J117">
-        <v>1026</v>
-      </c>
-    </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="118" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A118">
-        <v>1071</v>
+        <v>1082</v>
       </c>
       <c r="B118" s="1">
-        <v>45731</v>
+        <v>45832</v>
       </c>
       <c r="D118" s="1">
-        <v>45731</v>
+        <v>45832</v>
       </c>
       <c r="F118">
         <v>1</v>
       </c>
       <c r="J118">
-        <v>1071</v>
-      </c>
-    </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.45">
+        <v>1082</v>
+      </c>
+      <c r="K118" s="2">
+        <v>1083</v>
+      </c>
+      <c r="L118" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="119" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A119">
-        <v>1073</v>
+        <v>1085</v>
       </c>
       <c r="B119" s="1">
-        <v>45752</v>
-      </c>
-      <c r="C119" s="1">
-        <v>45892</v>
+        <v>45743</v>
       </c>
       <c r="D119" s="1">
-        <v>45752</v>
-      </c>
-      <c r="E119" s="1">
-        <v>45892</v>
+        <v>45743</v>
       </c>
       <c r="F119">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="J119">
+        <v>1085</v>
       </c>
       <c r="K119" s="2">
-        <v>1078</v>
+        <v>1084</v>
       </c>
       <c r="L119" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A120">
-        <v>1074</v>
-      </c>
-      <c r="B120" s="1">
-        <v>45762</v>
-      </c>
-      <c r="D120" s="1">
-        <v>45762</v>
-      </c>
-      <c r="F120">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A121">
-        <v>1077</v>
-      </c>
-      <c r="B121" s="1">
-        <v>45864</v>
-      </c>
-      <c r="D121" s="1">
-        <v>45864</v>
-      </c>
-      <c r="F121">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A122">
-        <v>1082</v>
-      </c>
-      <c r="B122" s="1">
-        <v>45832</v>
-      </c>
-      <c r="D122" s="1">
-        <v>45832</v>
-      </c>
-      <c r="F122">
-        <v>1</v>
-      </c>
-      <c r="J122">
-        <v>1082</v>
-      </c>
-      <c r="K122" s="2">
-        <v>1083</v>
-      </c>
-      <c r="L122" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A123">
-        <v>1085</v>
-      </c>
-      <c r="B123" s="1">
-        <v>45743</v>
-      </c>
-      <c r="D123" s="1">
-        <v>45743</v>
-      </c>
-      <c r="F123">
-        <v>0</v>
-      </c>
-      <c r="J123">
-        <v>1085</v>
-      </c>
-      <c r="K123" s="2">
-        <v>1084</v>
-      </c>
-      <c r="L123" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>